<commit_message>
Notas con actualización de tutorias.
</commit_message>
<xml_diff>
--- a/notasED/CalificacionesCod18demayo.xlsx
+++ b/notasED/CalificacionesCod18demayo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Drive\Konrad Lorenz\Asignaturas\2020-I\Estructuras de Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B16E2E-203C-490E-81C8-2AAD46131037}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C789A90-47EC-4DA1-85A1-537AB332AA7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calificaciones Grupo 1" sheetId="1" r:id="rId1"/>
@@ -637,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH26"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AE7" sqref="AE7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1373,11 +1373,11 @@
         <v>40</v>
       </c>
       <c r="AB7" s="14">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AC7" s="18">
         <f t="shared" si="4"/>
-        <v>62.900000000000006</v>
+        <v>67.900000000000006</v>
       </c>
       <c r="AD7" s="18">
         <f t="shared" si="5"/>
@@ -1385,7 +1385,7 @@
       </c>
       <c r="AE7" s="19">
         <f t="shared" si="6"/>
-        <v>12.900000000000006</v>
+        <v>17.900000000000006</v>
       </c>
       <c r="AF7" s="19">
         <v>40</v>
@@ -1991,15 +1991,15 @@
         <v>32</v>
       </c>
       <c r="AB13" s="14">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AC13" s="18">
         <f t="shared" si="4"/>
-        <v>42.4</v>
+        <v>45.4</v>
       </c>
       <c r="AD13" s="18">
         <f t="shared" si="5"/>
-        <v>42.4</v>
+        <v>45.4</v>
       </c>
       <c r="AE13" s="19">
         <f t="shared" si="6"/>
@@ -2011,7 +2011,7 @@
       <c r="AG13" s="19"/>
       <c r="AH13" s="18">
         <f t="shared" si="7"/>
-        <v>34.133333333333333</v>
+        <v>35.133333333333333</v>
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.3">
@@ -2101,11 +2101,11 @@
         <v>40</v>
       </c>
       <c r="AB14" s="14">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="AC14" s="18">
         <f t="shared" si="4"/>
-        <v>68.900000000000006</v>
+        <v>72.900000000000006</v>
       </c>
       <c r="AD14" s="18">
         <f t="shared" si="5"/>
@@ -2113,7 +2113,7 @@
       </c>
       <c r="AE14" s="19">
         <f t="shared" si="6"/>
-        <v>18.900000000000006</v>
+        <v>22.900000000000006</v>
       </c>
       <c r="AF14" s="19">
         <v>50</v>
@@ -2201,11 +2201,11 @@
         <v>45</v>
       </c>
       <c r="AB15" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AC15" s="18">
         <f t="shared" si="4"/>
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AD15" s="18">
         <f t="shared" si="5"/>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="AE15" s="19">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AF15" s="19">
         <v>0</v>
@@ -2311,15 +2311,15 @@
         <v>14</v>
       </c>
       <c r="AB16" s="14">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="AC16" s="18">
         <f t="shared" si="4"/>
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="AD16" s="18">
         <f t="shared" si="5"/>
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="AE16" s="19">
         <f t="shared" si="6"/>
@@ -2331,7 +2331,7 @@
       <c r="AG16" s="19"/>
       <c r="AH16" s="18">
         <f t="shared" si="7"/>
-        <v>32.333333333333336</v>
+        <v>33.666666666666664</v>
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.3">
@@ -2419,15 +2419,15 @@
         <v>13</v>
       </c>
       <c r="AB17" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC17" s="18">
         <f t="shared" si="4"/>
-        <v>36.599999999999994</v>
+        <v>37.599999999999994</v>
       </c>
       <c r="AD17" s="18">
         <f t="shared" si="5"/>
-        <v>36.599999999999994</v>
+        <v>37.599999999999994</v>
       </c>
       <c r="AE17" s="19">
         <f t="shared" si="6"/>
@@ -2439,7 +2439,7 @@
       <c r="AG17" s="19"/>
       <c r="AH17" s="18">
         <f t="shared" si="7"/>
-        <v>31.199999999999996</v>
+        <v>31.533333333333331</v>
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.3">
@@ -3133,19 +3133,19 @@
         <v>25</v>
       </c>
       <c r="AB24" s="14">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AC24" s="18">
         <f t="shared" si="4"/>
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AD24" s="18">
         <f t="shared" si="5"/>
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AE24" s="19">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF24" s="19">
         <v>40</v>
@@ -3153,7 +3153,7 @@
       <c r="AG24" s="19"/>
       <c r="AH24" s="18">
         <f t="shared" si="7"/>
-        <v>35.333333333333329</v>
+        <v>35.666666666666671</v>
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.3">
@@ -3361,8 +3361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E37ED78-914C-4768-B352-F7C1A3B9BD7F}">
   <dimension ref="A1:AH14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AE4" sqref="AE4"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AH20" sqref="AH20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3686,15 +3686,15 @@
         <v>0</v>
       </c>
       <c r="AB3" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AC3" s="18">
         <f t="shared" ref="AC3:AC13" si="4">AA3+X3+AB3</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AD3" s="19">
         <f t="shared" ref="AD3:AD13" si="5">IF(AC3&gt;50,50,AC3)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AE3" s="19">
         <f t="shared" ref="AE3:AE13" si="6">IF(AC3&gt;50,AC3-50,0)</f>
@@ -3706,7 +3706,7 @@
       <c r="AG3" s="19"/>
       <c r="AH3" s="18">
         <f t="shared" ref="AH3:AH13" si="7">(AD3*20)/60+(W3*18)/60+(AF3*6)/60+(AG3*16)/60</f>
-        <v>19.176666666666666</v>
+        <v>20.843333333333334</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.3">
@@ -3767,7 +3767,7 @@
       <c r="S4" s="8">
         <v>0</v>
       </c>
-      <c r="T4" s="10">
+      <c r="T4" s="6">
         <v>3.3</v>
       </c>
       <c r="U4" s="8">

</xml_diff>

<commit_message>
Notas a 18 de mayo de 2020. Actualización 2
</commit_message>
<xml_diff>
--- a/notasED/CalificacionesCod18demayo.xlsx
+++ b/notasED/CalificacionesCod18demayo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Drive\Konrad Lorenz\Asignaturas\2020-I\Estructuras de Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C789A90-47EC-4DA1-85A1-537AB332AA7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2814B394-A760-4C06-98A3-B4E058F0B1F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -637,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AE7" sqref="AE7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1324,7 +1324,7 @@
         <v>3</v>
       </c>
       <c r="M7" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N7" s="3">
         <v>13.9</v>
@@ -1352,7 +1352,7 @@
       </c>
       <c r="V7" s="10">
         <f t="shared" si="0"/>
-        <v>67.900000000000006</v>
+        <v>72.900000000000006</v>
       </c>
       <c r="W7" s="10">
         <f t="shared" si="1"/>
@@ -1360,7 +1360,7 @@
       </c>
       <c r="X7" s="10">
         <f t="shared" si="2"/>
-        <v>17.900000000000006</v>
+        <v>22.900000000000006</v>
       </c>
       <c r="Y7" s="14">
         <v>10</v>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="AC7" s="18">
         <f t="shared" si="4"/>
-        <v>67.900000000000006</v>
+        <v>72.900000000000006</v>
       </c>
       <c r="AD7" s="18">
         <f t="shared" si="5"/>
@@ -1385,7 +1385,7 @@
       </c>
       <c r="AE7" s="19">
         <f t="shared" si="6"/>
-        <v>17.900000000000006</v>
+        <v>22.900000000000006</v>
       </c>
       <c r="AF7" s="19">
         <v>40</v>
@@ -3361,8 +3361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E37ED78-914C-4768-B352-F7C1A3B9BD7F}">
   <dimension ref="A1:AH14"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AH20" sqref="AH20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>